<commit_message>
[docu] stage verslag updated + changlog [feature] commands door planner
</commit_message>
<xml_diff>
--- a/documentatie/inhoud/WerkExcel-Planning-berekeningen.xlsx
+++ b/documentatie/inhoud/WerkExcel-Planning-berekeningen.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2A6E20-C47C-492B-B84A-FC4D238F2487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5C025A-5A95-4BD9-8A87-8E6E3006CA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>TAAK</t>
   </si>
@@ -335,6 +335,27 @@
   </si>
   <si>
     <t>ja</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>end target</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>mm/step</t>
+  </si>
+  <si>
+    <t>step/mm</t>
+  </si>
+  <si>
+    <t>meetlint vanaf links</t>
   </si>
 </sst>
 </file>
@@ -900,7 +921,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1154,6 +1175,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1226,7 +1256,7 @@
     <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1524,18 +1554,21 @@
     <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -2515,50 +2548,50 @@
         <v>22</v>
       </c>
       <c r="C3" s="70"/>
-      <c r="D3" s="111">
+      <c r="D3" s="113">
         <f>DATE(2025, 9, 1)</f>
         <v>45901</v>
       </c>
-      <c r="E3" s="111"/>
+      <c r="E3" s="113"/>
       <c r="P3" s="88"/>
       <c r="AF3" s="88"/>
       <c r="AR3" s="88"/>
       <c r="AY3" s="87"/>
       <c r="BM3" s="88"/>
       <c r="BN3" s="87"/>
-      <c r="BO3" s="112" t="s">
+      <c r="BO3" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="BP3" s="112"/>
-      <c r="BQ3" s="112"/>
-      <c r="BR3" s="112"/>
-      <c r="BS3" s="112"/>
-      <c r="BT3" s="112"/>
-      <c r="BU3" s="112"/>
-      <c r="BV3" s="112"/>
-      <c r="BW3" s="112"/>
-      <c r="BX3" s="112"/>
-      <c r="BY3" s="112"/>
+      <c r="BP3" s="111"/>
+      <c r="BQ3" s="111"/>
+      <c r="BR3" s="111"/>
+      <c r="BS3" s="111"/>
+      <c r="BT3" s="111"/>
+      <c r="BU3" s="111"/>
+      <c r="BV3" s="111"/>
+      <c r="BW3" s="111"/>
+      <c r="BX3" s="111"/>
+      <c r="BY3" s="111"/>
       <c r="CA3" s="88"/>
       <c r="CG3" s="87"/>
       <c r="CO3" s="88"/>
       <c r="DC3" s="88"/>
-      <c r="DP3" s="113" t="s">
+      <c r="DP3" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="DQ3" s="113"/>
-      <c r="DR3" s="113"/>
-      <c r="DS3" s="113"/>
-      <c r="DT3" s="113"/>
-      <c r="DU3" s="113"/>
-      <c r="DV3" s="113"/>
-      <c r="DW3" s="113"/>
-      <c r="DX3" s="113"/>
-      <c r="DY3" s="113"/>
-      <c r="DZ3" s="113"/>
-      <c r="EA3" s="113"/>
-      <c r="EB3" s="113"/>
-      <c r="EC3" s="113"/>
+      <c r="DQ3" s="112"/>
+      <c r="DR3" s="112"/>
+      <c r="DS3" s="112"/>
+      <c r="DT3" s="112"/>
+      <c r="DU3" s="112"/>
+      <c r="DV3" s="112"/>
+      <c r="DW3" s="112"/>
+      <c r="DX3" s="112"/>
+      <c r="DY3" s="112"/>
+      <c r="DZ3" s="112"/>
+      <c r="EA3" s="112"/>
+      <c r="EB3" s="112"/>
+      <c r="EC3" s="112"/>
       <c r="EZ3" s="88"/>
       <c r="FC3" s="87"/>
       <c r="FF3" s="87"/>
@@ -15028,6 +15061,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
+    <mergeCell ref="BL4:BR4"/>
     <mergeCell ref="EY4:FE4"/>
     <mergeCell ref="FF4:FL4"/>
     <mergeCell ref="FM4:FS4"/>
@@ -15044,18 +15089,6 @@
     <mergeCell ref="DP4:DV4"/>
     <mergeCell ref="DW4:EC4"/>
     <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="BL4:BR4"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <conditionalFormatting sqref="C7:C59">
@@ -15228,10 +15261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E16046-3957-429D-BA41-59B4EEE9D413}">
-  <dimension ref="B5:I37"/>
+  <dimension ref="A5:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15688,7 +15721,7 @@
         <v>2.3230615159823349E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>11</v>
       </c>
@@ -15705,7 +15738,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>12</v>
       </c>
@@ -15722,7 +15755,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>13</v>
       </c>
@@ -15739,7 +15772,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>14</v>
       </c>
@@ -15756,7 +15789,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>15</v>
       </c>
@@ -15771,6 +15804,362 @@
       <c r="G37" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>98</v>
+      </c>
+      <c r="G42" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" t="s">
+        <v>100</v>
+      </c>
+      <c r="I42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>999</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f>D43-E43</f>
+        <v>997</v>
+      </c>
+      <c r="H43">
+        <f>C43/G43</f>
+        <v>2.0060180541624874E-2</v>
+      </c>
+      <c r="I43">
+        <f>G43/C43</f>
+        <v>49.85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="115"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115">
+        <v>165</v>
+      </c>
+      <c r="D44" s="115">
+        <v>2</v>
+      </c>
+      <c r="E44" s="115">
+        <v>9997</v>
+      </c>
+      <c r="F44" s="115">
+        <v>10000</v>
+      </c>
+      <c r="G44" s="115">
+        <f>E44-D44</f>
+        <v>9995</v>
+      </c>
+      <c r="H44" s="115">
+        <f>C44/G44</f>
+        <v>1.6508254127063533E-2</v>
+      </c>
+      <c r="I44" s="115">
+        <f t="shared" ref="I44:I55" si="6">G44/C44</f>
+        <v>60.575757575757578</v>
+      </c>
+      <c r="J44" s="115"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="115"/>
+      <c r="M44" s="115"/>
+      <c r="N44" s="115"/>
+      <c r="O44" s="115"/>
+      <c r="P44" s="115"/>
+      <c r="Q44" s="115"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" s="117" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="117"/>
+      <c r="C45" s="117">
+        <v>500</v>
+      </c>
+      <c r="D45" s="117">
+        <v>2</v>
+      </c>
+      <c r="E45" s="117">
+        <v>-30002</v>
+      </c>
+      <c r="F45" s="117">
+        <v>-30000</v>
+      </c>
+      <c r="G45" s="117">
+        <f>D45-E45</f>
+        <v>30004</v>
+      </c>
+      <c r="H45" s="117">
+        <f>C45/G45</f>
+        <v>1.666444474070124E-2</v>
+      </c>
+      <c r="I45" s="117">
+        <f t="shared" si="6"/>
+        <v>60.008000000000003</v>
+      </c>
+      <c r="J45" s="117"/>
+      <c r="K45" s="117"/>
+      <c r="L45" s="117"/>
+      <c r="M45" s="117"/>
+      <c r="N45" s="117"/>
+      <c r="O45" s="117"/>
+      <c r="P45" s="117"/>
+      <c r="Q45" s="117"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C46" s="115">
+        <v>165</v>
+      </c>
+      <c r="D46" s="115">
+        <v>0</v>
+      </c>
+      <c r="E46" s="115">
+        <v>9996</v>
+      </c>
+      <c r="F46" s="115">
+        <v>10000</v>
+      </c>
+      <c r="G46" s="115">
+        <f>E46</f>
+        <v>9996</v>
+      </c>
+      <c r="H46" s="115">
+        <f>C46/G46</f>
+        <v>1.6506602641056422E-2</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="6"/>
+        <v>60.581818181818178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C47" s="115">
+        <v>498</v>
+      </c>
+      <c r="D47" s="115">
+        <v>0</v>
+      </c>
+      <c r="E47" s="115">
+        <v>30001</v>
+      </c>
+      <c r="F47" s="115">
+        <v>30000</v>
+      </c>
+      <c r="G47" s="115">
+        <f>E47</f>
+        <v>30001</v>
+      </c>
+      <c r="H47" s="115">
+        <f>C47/G47</f>
+        <v>1.6599446685110496E-2</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="6"/>
+        <v>60.242971887550198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C48" s="115">
+        <v>997</v>
+      </c>
+      <c r="D48" s="116">
+        <v>0</v>
+      </c>
+      <c r="E48" s="116">
+        <v>60000</v>
+      </c>
+      <c r="F48" s="116">
+        <v>60000</v>
+      </c>
+      <c r="G48" s="115">
+        <v>60000</v>
+      </c>
+      <c r="H48" s="115">
+        <f>C48/G48</f>
+        <v>1.6616666666666665E-2</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="6"/>
+        <v>60.180541624874621</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C49" s="116">
+        <v>167</v>
+      </c>
+      <c r="D49" s="116">
+        <v>0</v>
+      </c>
+      <c r="E49" s="116">
+        <v>9998</v>
+      </c>
+      <c r="F49" s="116">
+        <v>10000</v>
+      </c>
+      <c r="G49" s="115">
+        <f>E49</f>
+        <v>9998</v>
+      </c>
+      <c r="H49" s="115">
+        <f>C49/G49</f>
+        <v>1.6703340668133625E-2</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="6"/>
+        <v>59.868263473053894</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C50" s="116">
+        <v>167</v>
+      </c>
+      <c r="D50" s="116">
+        <v>0</v>
+      </c>
+      <c r="E50" s="116">
+        <v>9998</v>
+      </c>
+      <c r="F50" s="116">
+        <v>10000</v>
+      </c>
+      <c r="G50" s="115">
+        <f>E50</f>
+        <v>9998</v>
+      </c>
+      <c r="H50" s="115">
+        <f>C50/G50</f>
+        <v>1.6703340668133625E-2</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="6"/>
+        <v>59.868263473053894</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C51" s="116">
+        <v>499</v>
+      </c>
+      <c r="D51" s="116">
+        <v>0</v>
+      </c>
+      <c r="E51" s="116">
+        <v>30000</v>
+      </c>
+      <c r="F51" s="116">
+        <v>30000</v>
+      </c>
+      <c r="G51" s="116">
+        <f>E51</f>
+        <v>30000</v>
+      </c>
+      <c r="H51" s="115">
+        <f t="shared" ref="H51:H54" si="7">C51/G51</f>
+        <v>1.6633333333333333E-2</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="6"/>
+        <v>60.120240480961925</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C52" s="116">
+        <v>499</v>
+      </c>
+      <c r="D52" s="116">
+        <v>0</v>
+      </c>
+      <c r="E52" s="116">
+        <v>29999</v>
+      </c>
+      <c r="F52" s="116">
+        <v>30000</v>
+      </c>
+      <c r="G52" s="116">
+        <f>E52</f>
+        <v>29999</v>
+      </c>
+      <c r="H52" s="115">
+        <f t="shared" si="7"/>
+        <v>1.6633887796259874E-2</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="6"/>
+        <v>60.118236472945888</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C53" s="116">
+        <v>997</v>
+      </c>
+      <c r="D53" s="116">
+        <v>0</v>
+      </c>
+      <c r="E53" s="116">
+        <v>60002</v>
+      </c>
+      <c r="F53" s="116">
+        <v>60000</v>
+      </c>
+      <c r="G53" s="116">
+        <f>E53</f>
+        <v>60002</v>
+      </c>
+      <c r="H53" s="115">
+        <f t="shared" si="7"/>
+        <v>1.6616112796240125E-2</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="6"/>
+        <v>60.182547642928789</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C54" s="116">
+        <v>996</v>
+      </c>
+      <c r="D54" s="116">
+        <v>0</v>
+      </c>
+      <c r="E54" s="116">
+        <v>59999</v>
+      </c>
+      <c r="F54" s="116">
+        <v>60000</v>
+      </c>
+      <c r="G54" s="116">
+        <f>E54</f>
+        <v>59999</v>
+      </c>
+      <c r="H54" s="115">
+        <f t="shared" si="7"/>
+        <v>1.6600276671277853E-2</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="6"/>
+        <v>60.239959839357432</v>
       </c>
     </row>
   </sheetData>
@@ -15885,35 +16274,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16201,27 +16561,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16240,4 +16609,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
opleverset aangemaakt, stageverslag verbeterd
</commit_message>
<xml_diff>
--- a/documentatie/inhoud/WerkExcel-Planning-berekeningen.xlsx
+++ b/documentatie/inhoud/WerkExcel-Planning-berekeningen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65778055-BB97-4000-A6C8-671B583E1D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17720DD4-85CF-42B0-B987-B4394797119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlanning" sheetId="11" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="115">
   <si>
     <t>TAAK</t>
   </si>
@@ -355,9 +355,6 @@
     <t>meetlint vanaf links</t>
   </si>
   <si>
-    <t>CNC uitzoeken</t>
-  </si>
-  <si>
     <t>bracket ontwerpen</t>
   </si>
   <si>
@@ -411,7 +408,7 @@
     <numFmt numFmtId="170" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="171" formatCode="d"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
   </numFmts>
   <fonts count="35" x14ac:knownFonts="1">
     <font>
@@ -1588,6 +1585,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1597,20 +1596,18 @@
     <xf numFmtId="170" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -3410,9 +3407,9 @@
   </sheetPr>
   <dimension ref="A1:GC78"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="CC1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="FA12" sqref="FA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3504,50 +3501,50 @@
         <v>22</v>
       </c>
       <c r="C3" s="70"/>
-      <c r="D3" s="114">
+      <c r="D3" s="118">
         <f>DATE(2025, 9, 1)</f>
         <v>45901</v>
       </c>
-      <c r="E3" s="114"/>
+      <c r="E3" s="118"/>
       <c r="P3" s="88"/>
       <c r="AF3" s="88"/>
       <c r="AR3" s="88"/>
       <c r="AY3" s="87"/>
       <c r="BM3" s="88"/>
       <c r="BN3" s="87"/>
-      <c r="BO3" s="115" t="s">
+      <c r="BO3" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="BP3" s="115"/>
-      <c r="BQ3" s="115"/>
-      <c r="BR3" s="115"/>
-      <c r="BS3" s="115"/>
-      <c r="BT3" s="115"/>
-      <c r="BU3" s="115"/>
-      <c r="BV3" s="115"/>
-      <c r="BW3" s="115"/>
-      <c r="BX3" s="115"/>
-      <c r="BY3" s="115"/>
+      <c r="BP3" s="116"/>
+      <c r="BQ3" s="116"/>
+      <c r="BR3" s="116"/>
+      <c r="BS3" s="116"/>
+      <c r="BT3" s="116"/>
+      <c r="BU3" s="116"/>
+      <c r="BV3" s="116"/>
+      <c r="BW3" s="116"/>
+      <c r="BX3" s="116"/>
+      <c r="BY3" s="116"/>
       <c r="CA3" s="88"/>
       <c r="CG3" s="87"/>
       <c r="CO3" s="88"/>
       <c r="DC3" s="88"/>
-      <c r="DP3" s="116" t="s">
+      <c r="DP3" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="DQ3" s="116"/>
-      <c r="DR3" s="116"/>
-      <c r="DS3" s="116"/>
-      <c r="DT3" s="116"/>
-      <c r="DU3" s="116"/>
-      <c r="DV3" s="116"/>
-      <c r="DW3" s="116"/>
-      <c r="DX3" s="116"/>
-      <c r="DY3" s="116"/>
-      <c r="DZ3" s="116"/>
-      <c r="EA3" s="116"/>
-      <c r="EB3" s="116"/>
-      <c r="EC3" s="116"/>
+      <c r="DQ3" s="117"/>
+      <c r="DR3" s="117"/>
+      <c r="DS3" s="117"/>
+      <c r="DT3" s="117"/>
+      <c r="DU3" s="117"/>
+      <c r="DV3" s="117"/>
+      <c r="DW3" s="117"/>
+      <c r="DX3" s="117"/>
+      <c r="DY3" s="117"/>
+      <c r="DZ3" s="117"/>
+      <c r="EA3" s="117"/>
+      <c r="EB3" s="117"/>
+      <c r="EC3" s="117"/>
       <c r="EZ3" s="88"/>
       <c r="FC3" s="87"/>
       <c r="FF3" s="87"/>
@@ -3560,256 +3557,256 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="113">
         <f>H5</f>
         <v>45901</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="111">
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="113">
         <f>O5</f>
         <v>45908</v>
       </c>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="111">
+      <c r="P4" s="114"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="113">
         <f>V5</f>
         <v>45915</v>
       </c>
-      <c r="W4" s="112"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="112"/>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="113"/>
-      <c r="AC4" s="111">
+      <c r="W4" s="114"/>
+      <c r="X4" s="114"/>
+      <c r="Y4" s="114"/>
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="113">
         <f>AC5</f>
         <v>45922</v>
       </c>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="112"/>
-      <c r="AF4" s="112"/>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="113"/>
-      <c r="AJ4" s="111">
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="114"/>
+      <c r="AF4" s="114"/>
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="113">
         <f>AJ5</f>
         <v>45929</v>
       </c>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="112"/>
-      <c r="AM4" s="112"/>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="113"/>
-      <c r="AQ4" s="111">
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="114"/>
+      <c r="AM4" s="114"/>
+      <c r="AN4" s="114"/>
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="113">
         <f>AQ5</f>
         <v>45936</v>
       </c>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="112"/>
-      <c r="AT4" s="112"/>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="113"/>
-      <c r="AX4" s="111">
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="114"/>
+      <c r="AT4" s="114"/>
+      <c r="AU4" s="114"/>
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="113">
         <f>AX5</f>
         <v>45943</v>
       </c>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="112"/>
-      <c r="BA4" s="112"/>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="113"/>
-      <c r="BE4" s="111">
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="114"/>
+      <c r="BA4" s="114"/>
+      <c r="BB4" s="114"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="113">
         <f>BE5</f>
         <v>45950</v>
       </c>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="112"/>
-      <c r="BH4" s="112"/>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="113"/>
-      <c r="BL4" s="111">
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="114"/>
+      <c r="BH4" s="114"/>
+      <c r="BI4" s="114"/>
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="115"/>
+      <c r="BL4" s="113">
         <f>BL5</f>
         <v>45957</v>
       </c>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="112"/>
-      <c r="BO4" s="112"/>
-      <c r="BP4" s="112"/>
-      <c r="BQ4" s="112"/>
-      <c r="BR4" s="113"/>
-      <c r="BS4" s="111">
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="114"/>
+      <c r="BO4" s="114"/>
+      <c r="BP4" s="114"/>
+      <c r="BQ4" s="114"/>
+      <c r="BR4" s="115"/>
+      <c r="BS4" s="113">
         <f>BS5</f>
         <v>45964</v>
       </c>
-      <c r="BT4" s="112"/>
-      <c r="BU4" s="112"/>
-      <c r="BV4" s="112"/>
-      <c r="BW4" s="112"/>
-      <c r="BX4" s="112"/>
-      <c r="BY4" s="113"/>
-      <c r="BZ4" s="111">
+      <c r="BT4" s="114"/>
+      <c r="BU4" s="114"/>
+      <c r="BV4" s="114"/>
+      <c r="BW4" s="114"/>
+      <c r="BX4" s="114"/>
+      <c r="BY4" s="115"/>
+      <c r="BZ4" s="113">
         <f>BZ5</f>
         <v>45971</v>
       </c>
-      <c r="CA4" s="112"/>
-      <c r="CB4" s="112"/>
-      <c r="CC4" s="112"/>
-      <c r="CD4" s="112"/>
-      <c r="CE4" s="112"/>
-      <c r="CF4" s="113"/>
-      <c r="CG4" s="111">
+      <c r="CA4" s="114"/>
+      <c r="CB4" s="114"/>
+      <c r="CC4" s="114"/>
+      <c r="CD4" s="114"/>
+      <c r="CE4" s="114"/>
+      <c r="CF4" s="115"/>
+      <c r="CG4" s="113">
         <f>CG5</f>
         <v>45978</v>
       </c>
-      <c r="CH4" s="112"/>
-      <c r="CI4" s="112"/>
-      <c r="CJ4" s="112"/>
-      <c r="CK4" s="112"/>
-      <c r="CL4" s="112"/>
-      <c r="CM4" s="113"/>
-      <c r="CN4" s="111">
+      <c r="CH4" s="114"/>
+      <c r="CI4" s="114"/>
+      <c r="CJ4" s="114"/>
+      <c r="CK4" s="114"/>
+      <c r="CL4" s="114"/>
+      <c r="CM4" s="115"/>
+      <c r="CN4" s="113">
         <f>CN5</f>
         <v>45985</v>
       </c>
-      <c r="CO4" s="112"/>
-      <c r="CP4" s="112"/>
-      <c r="CQ4" s="112"/>
-      <c r="CR4" s="112"/>
-      <c r="CS4" s="112"/>
-      <c r="CT4" s="113"/>
-      <c r="CU4" s="111">
+      <c r="CO4" s="114"/>
+      <c r="CP4" s="114"/>
+      <c r="CQ4" s="114"/>
+      <c r="CR4" s="114"/>
+      <c r="CS4" s="114"/>
+      <c r="CT4" s="115"/>
+      <c r="CU4" s="113">
         <f>CU5</f>
         <v>45992</v>
       </c>
-      <c r="CV4" s="112"/>
-      <c r="CW4" s="112"/>
-      <c r="CX4" s="112"/>
-      <c r="CY4" s="112"/>
-      <c r="CZ4" s="112"/>
-      <c r="DA4" s="113"/>
-      <c r="DB4" s="111">
+      <c r="CV4" s="114"/>
+      <c r="CW4" s="114"/>
+      <c r="CX4" s="114"/>
+      <c r="CY4" s="114"/>
+      <c r="CZ4" s="114"/>
+      <c r="DA4" s="115"/>
+      <c r="DB4" s="113">
         <f t="shared" ref="DB4" si="0">DB5</f>
         <v>45999</v>
       </c>
-      <c r="DC4" s="112"/>
-      <c r="DD4" s="112"/>
-      <c r="DE4" s="112"/>
-      <c r="DF4" s="112"/>
-      <c r="DG4" s="112"/>
-      <c r="DH4" s="113"/>
-      <c r="DI4" s="111">
+      <c r="DC4" s="114"/>
+      <c r="DD4" s="114"/>
+      <c r="DE4" s="114"/>
+      <c r="DF4" s="114"/>
+      <c r="DG4" s="114"/>
+      <c r="DH4" s="115"/>
+      <c r="DI4" s="113">
         <f t="shared" ref="DI4" si="1">DI5</f>
         <v>46006</v>
       </c>
-      <c r="DJ4" s="112"/>
-      <c r="DK4" s="112"/>
-      <c r="DL4" s="112"/>
-      <c r="DM4" s="112"/>
-      <c r="DN4" s="112"/>
-      <c r="DO4" s="113"/>
-      <c r="DP4" s="111">
+      <c r="DJ4" s="114"/>
+      <c r="DK4" s="114"/>
+      <c r="DL4" s="114"/>
+      <c r="DM4" s="114"/>
+      <c r="DN4" s="114"/>
+      <c r="DO4" s="115"/>
+      <c r="DP4" s="113">
         <f t="shared" ref="DP4" si="2">DP5</f>
         <v>46013</v>
       </c>
-      <c r="DQ4" s="112"/>
-      <c r="DR4" s="112"/>
-      <c r="DS4" s="112"/>
-      <c r="DT4" s="112"/>
-      <c r="DU4" s="112"/>
-      <c r="DV4" s="113"/>
-      <c r="DW4" s="111">
+      <c r="DQ4" s="114"/>
+      <c r="DR4" s="114"/>
+      <c r="DS4" s="114"/>
+      <c r="DT4" s="114"/>
+      <c r="DU4" s="114"/>
+      <c r="DV4" s="115"/>
+      <c r="DW4" s="113">
         <f t="shared" ref="DW4" si="3">DW5</f>
         <v>46020</v>
       </c>
-      <c r="DX4" s="112"/>
-      <c r="DY4" s="112"/>
-      <c r="DZ4" s="112"/>
-      <c r="EA4" s="112"/>
-      <c r="EB4" s="112"/>
-      <c r="EC4" s="113"/>
-      <c r="ED4" s="111">
+      <c r="DX4" s="114"/>
+      <c r="DY4" s="114"/>
+      <c r="DZ4" s="114"/>
+      <c r="EA4" s="114"/>
+      <c r="EB4" s="114"/>
+      <c r="EC4" s="115"/>
+      <c r="ED4" s="113">
         <f t="shared" ref="ED4" si="4">ED5</f>
         <v>46027</v>
       </c>
-      <c r="EE4" s="112"/>
-      <c r="EF4" s="112"/>
-      <c r="EG4" s="112"/>
-      <c r="EH4" s="112"/>
-      <c r="EI4" s="112"/>
-      <c r="EJ4" s="113"/>
-      <c r="EK4" s="111">
+      <c r="EE4" s="114"/>
+      <c r="EF4" s="114"/>
+      <c r="EG4" s="114"/>
+      <c r="EH4" s="114"/>
+      <c r="EI4" s="114"/>
+      <c r="EJ4" s="115"/>
+      <c r="EK4" s="113">
         <f t="shared" ref="EK4" si="5">EK5</f>
         <v>46034</v>
       </c>
-      <c r="EL4" s="112"/>
-      <c r="EM4" s="112"/>
-      <c r="EN4" s="112"/>
-      <c r="EO4" s="112"/>
-      <c r="EP4" s="112"/>
-      <c r="EQ4" s="113"/>
-      <c r="ER4" s="111">
+      <c r="EL4" s="114"/>
+      <c r="EM4" s="114"/>
+      <c r="EN4" s="114"/>
+      <c r="EO4" s="114"/>
+      <c r="EP4" s="114"/>
+      <c r="EQ4" s="115"/>
+      <c r="ER4" s="113">
         <f t="shared" ref="ER4" si="6">ER5</f>
         <v>46041</v>
       </c>
-      <c r="ES4" s="112"/>
-      <c r="ET4" s="112"/>
-      <c r="EU4" s="112"/>
-      <c r="EV4" s="112"/>
-      <c r="EW4" s="112"/>
-      <c r="EX4" s="113"/>
-      <c r="EY4" s="111">
+      <c r="ES4" s="114"/>
+      <c r="ET4" s="114"/>
+      <c r="EU4" s="114"/>
+      <c r="EV4" s="114"/>
+      <c r="EW4" s="114"/>
+      <c r="EX4" s="115"/>
+      <c r="EY4" s="113">
         <f t="shared" ref="EY4" si="7">EY5</f>
         <v>46048</v>
       </c>
-      <c r="EZ4" s="112"/>
-      <c r="FA4" s="112"/>
-      <c r="FB4" s="112"/>
-      <c r="FC4" s="112"/>
-      <c r="FD4" s="112"/>
-      <c r="FE4" s="113"/>
-      <c r="FF4" s="111">
+      <c r="EZ4" s="114"/>
+      <c r="FA4" s="114"/>
+      <c r="FB4" s="114"/>
+      <c r="FC4" s="114"/>
+      <c r="FD4" s="114"/>
+      <c r="FE4" s="115"/>
+      <c r="FF4" s="113">
         <f t="shared" ref="FF4" si="8">FF5</f>
         <v>46055</v>
       </c>
-      <c r="FG4" s="112"/>
-      <c r="FH4" s="112"/>
-      <c r="FI4" s="112"/>
-      <c r="FJ4" s="112"/>
-      <c r="FK4" s="112"/>
-      <c r="FL4" s="113"/>
-      <c r="FM4" s="111">
+      <c r="FG4" s="114"/>
+      <c r="FH4" s="114"/>
+      <c r="FI4" s="114"/>
+      <c r="FJ4" s="114"/>
+      <c r="FK4" s="114"/>
+      <c r="FL4" s="115"/>
+      <c r="FM4" s="113">
         <f t="shared" ref="FM4" si="9">FM5</f>
         <v>46062</v>
       </c>
-      <c r="FN4" s="112"/>
-      <c r="FO4" s="112"/>
-      <c r="FP4" s="112"/>
-      <c r="FQ4" s="112"/>
-      <c r="FR4" s="112"/>
-      <c r="FS4" s="113"/>
-      <c r="FT4" s="111">
+      <c r="FN4" s="114"/>
+      <c r="FO4" s="114"/>
+      <c r="FP4" s="114"/>
+      <c r="FQ4" s="114"/>
+      <c r="FR4" s="114"/>
+      <c r="FS4" s="115"/>
+      <c r="FT4" s="113">
         <f t="shared" ref="FT4" si="10">FT5</f>
         <v>46069</v>
       </c>
-      <c r="FU4" s="112"/>
-      <c r="FV4" s="112"/>
-      <c r="FW4" s="112"/>
-      <c r="FX4" s="112"/>
-      <c r="FY4" s="112"/>
-      <c r="FZ4" s="113"/>
+      <c r="FU4" s="114"/>
+      <c r="FV4" s="114"/>
+      <c r="FW4" s="114"/>
+      <c r="FX4" s="114"/>
+      <c r="FY4" s="114"/>
+      <c r="FZ4" s="115"/>
       <c r="GC4" s="92">
         <v>1</v>
       </c>
@@ -5819,7 +5816,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="77">
         <f>DATE(2026,1,12)</f>
@@ -6211,7 +6208,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="76">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D12" s="77">
         <f>DATE(2026,1,1)</f>
@@ -6407,15 +6404,15 @@
         <v>32</v>
       </c>
       <c r="C13" s="76">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D13" s="77">
         <f>DATE(2026, 1, 1)</f>
         <v>46023</v>
       </c>
       <c r="E13" s="77">
-        <f>DATE(2026, 1, 25)</f>
-        <v>46047</v>
+        <f>DATE(2026, 1, 29)</f>
+        <v>46051</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -6990,7 +6987,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D16" s="57">
         <v>45902</v>
@@ -7573,12 +7570,8 @@
     </row>
     <row r="19" spans="1:185" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="40"/>
-      <c r="B19" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="57"/>
       <c r="E19" s="57"/>
       <c r="F19" s="27"/>
@@ -7768,7 +7761,7 @@
         <v>72</v>
       </c>
       <c r="C20" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D20" s="57">
         <v>45909</v>
@@ -8936,10 +8929,14 @@
         <v>75</v>
       </c>
       <c r="C26" s="17">
-        <v>0</v>
-      </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="60">
+        <v>45992</v>
+      </c>
+      <c r="E26" s="60">
+        <v>46004</v>
+      </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -10873,16 +10870,16 @@
     <row r="36" spans="1:185" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="40"/>
       <c r="B36" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D36" s="63">
         <v>46010</v>
       </c>
       <c r="E36" s="63">
-        <v>46027</v>
+        <v>46041</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
@@ -11066,7 +11063,7 @@
     <row r="37" spans="1:185" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="40"/>
       <c r="B37" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="20">
         <v>1</v>
@@ -11259,10 +11256,10 @@
     <row r="38" spans="1:185" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="40"/>
       <c r="B38" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="63">
         <v>46027</v>
@@ -12222,7 +12219,7 @@
         <v>76</v>
       </c>
       <c r="C43" s="23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D43" s="66">
         <v>45901</v>
@@ -12415,9 +12412,7 @@
       <c r="A44" s="40"/>
       <c r="B44" s="49"/>
       <c r="C44" s="23"/>
-      <c r="D44" s="66">
-        <v>45901</v>
-      </c>
+      <c r="D44" s="66"/>
       <c r="E44" s="66"/>
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
@@ -16608,6 +16603,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
+    <mergeCell ref="BL4:BR4"/>
     <mergeCell ref="EY4:FE4"/>
     <mergeCell ref="FF4:FL4"/>
     <mergeCell ref="FM4:FS4"/>
@@ -16624,18 +16631,6 @@
     <mergeCell ref="DP4:DV4"/>
     <mergeCell ref="DW4:EC4"/>
     <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="BL4:BR4"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <conditionalFormatting sqref="C7:C62">
@@ -16767,7 +16762,7 @@
       <formula>AND(task_end&gt;=FT$5,task_start&lt;GP$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Weergegeven week" prompt="Als u dit getal wijzigt, scrolt u door de weergave van het Gantt-diagram." sqref="D4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -16810,8 +16805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E16046-3957-429D-BA41-59B4EEE9D413}">
   <dimension ref="A5:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L74" sqref="L74"/>
+    <sheetView topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16821,13 +16816,13 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -17269,91 +17264,6 @@
         <v>2.3230615159823349E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>11</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G33" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B34">
-        <v>12</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G34" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>13</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G35" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>14</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G36" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <v>15</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G37" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>81</v>
@@ -17427,7 +17337,7 @@
         <v>1.6508254127063533E-2</v>
       </c>
       <c r="I44" s="108">
-        <f t="shared" ref="I44:I54" si="7">G44/C44</f>
+        <f t="shared" ref="I44:I53" si="7">G44/C44</f>
         <v>60.575757575757578</v>
       </c>
       <c r="J44" s="108"/>
@@ -17712,27 +17622,27 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>107</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>108</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>109</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>110</v>
-      </c>
-      <c r="G56" t="s">
-        <v>111</v>
       </c>
       <c r="H56" t="s">
         <v>99</v>
@@ -17748,10 +17658,10 @@
       <c r="D57">
         <v>145.5</v>
       </c>
-      <c r="E57" s="119">
+      <c r="E57" s="112">
         <v>134.30000000000001</v>
       </c>
-      <c r="F57" s="119">
+      <c r="F57" s="112">
         <f>D57-E57</f>
         <v>11.199999999999989</v>
       </c>
@@ -17759,11 +17669,11 @@
         <f>F57/C57*1000</f>
         <v>11.199999999999989</v>
       </c>
-      <c r="H57" s="118">
+      <c r="H57" s="111">
         <f>(F57*10)/C57</f>
         <v>0.11199999999999989</v>
       </c>
-      <c r="I57" s="118">
+      <c r="I57" s="111">
         <f>C57/(F57*10)</f>
         <v>8.9285714285714377</v>
       </c>
@@ -17775,10 +17685,10 @@
       <c r="D58">
         <v>145.5</v>
       </c>
-      <c r="E58" s="119">
+      <c r="E58" s="112">
         <v>130</v>
       </c>
-      <c r="F58" s="119">
+      <c r="F58" s="112">
         <f t="shared" ref="F58:F71" si="10">D58-E58</f>
         <v>15.5</v>
       </c>
@@ -17786,11 +17696,11 @@
         <f t="shared" ref="G58:G71" si="11">F58/C58*1000</f>
         <v>15.5</v>
       </c>
-      <c r="H58" s="118">
+      <c r="H58" s="111">
         <f t="shared" ref="H58:H71" si="12">(F58*10)/C58</f>
         <v>0.155</v>
       </c>
-      <c r="I58" s="118">
+      <c r="I58" s="111">
         <f t="shared" ref="I58:I70" si="13">C58/(F58*10)</f>
         <v>6.4516129032258061</v>
       </c>
@@ -17802,10 +17712,10 @@
       <c r="D59">
         <v>145.5</v>
       </c>
-      <c r="E59" s="119">
+      <c r="E59" s="112">
         <v>125.5</v>
       </c>
-      <c r="F59" s="119">
+      <c r="F59" s="112">
         <f t="shared" si="10"/>
         <v>20</v>
       </c>
@@ -17813,11 +17723,11 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="H59" s="118">
+      <c r="H59" s="111">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="I59" s="118">
+      <c r="I59" s="111">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
@@ -17829,10 +17739,10 @@
       <c r="D60">
         <v>145.5</v>
       </c>
-      <c r="E60" s="119">
+      <c r="E60" s="112">
         <v>125.5</v>
       </c>
-      <c r="F60" s="119">
+      <c r="F60" s="112">
         <f t="shared" si="10"/>
         <v>20</v>
       </c>
@@ -17840,11 +17750,11 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="H60" s="118">
+      <c r="H60" s="111">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="I60" s="118">
+      <c r="I60" s="111">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
@@ -17856,10 +17766,10 @@
       <c r="D61">
         <v>145.5</v>
       </c>
-      <c r="E61" s="119">
+      <c r="E61" s="112">
         <v>125.6</v>
       </c>
-      <c r="F61" s="119">
+      <c r="F61" s="112">
         <f t="shared" si="10"/>
         <v>19.900000000000006</v>
       </c>
@@ -17867,11 +17777,11 @@
         <f t="shared" si="11"/>
         <v>19.900000000000006</v>
       </c>
-      <c r="H61" s="118">
+      <c r="H61" s="111">
         <f t="shared" si="12"/>
         <v>0.19900000000000007</v>
       </c>
-      <c r="I61" s="118">
+      <c r="I61" s="111">
         <f t="shared" si="13"/>
         <v>5.0251256281407022</v>
       </c>
@@ -17883,10 +17793,10 @@
       <c r="D62">
         <v>145.5</v>
       </c>
-      <c r="E62" s="119">
+      <c r="E62" s="112">
         <v>106</v>
       </c>
-      <c r="F62" s="119">
+      <c r="F62" s="112">
         <f t="shared" si="10"/>
         <v>39.5</v>
       </c>
@@ -17894,11 +17804,11 @@
         <f t="shared" si="11"/>
         <v>19.75</v>
       </c>
-      <c r="H62" s="118">
+      <c r="H62" s="111">
         <f t="shared" si="12"/>
         <v>0.19750000000000001</v>
       </c>
-      <c r="I62" s="118">
+      <c r="I62" s="111">
         <f t="shared" si="13"/>
         <v>5.0632911392405067</v>
       </c>
@@ -17910,10 +17820,10 @@
       <c r="D63">
         <v>145.5</v>
       </c>
-      <c r="E63" s="119">
+      <c r="E63" s="112">
         <v>106.5</v>
       </c>
-      <c r="F63" s="119">
+      <c r="F63" s="112">
         <f t="shared" si="10"/>
         <v>39</v>
       </c>
@@ -17921,11 +17831,11 @@
         <f t="shared" si="11"/>
         <v>19.5</v>
       </c>
-      <c r="H63" s="118">
+      <c r="H63" s="111">
         <f t="shared" si="12"/>
         <v>0.19500000000000001</v>
       </c>
-      <c r="I63" s="118">
+      <c r="I63" s="111">
         <f t="shared" si="13"/>
         <v>5.1282051282051286</v>
       </c>
@@ -17937,10 +17847,10 @@
       <c r="D64">
         <v>145.5</v>
       </c>
-      <c r="E64" s="119">
+      <c r="E64" s="112">
         <v>106</v>
       </c>
-      <c r="F64" s="119">
+      <c r="F64" s="112">
         <f t="shared" si="10"/>
         <v>39.5</v>
       </c>
@@ -17948,11 +17858,11 @@
         <f t="shared" si="11"/>
         <v>19.75</v>
       </c>
-      <c r="H64" s="118">
+      <c r="H64" s="111">
         <f t="shared" si="12"/>
         <v>0.19750000000000001</v>
       </c>
-      <c r="I64" s="118">
+      <c r="I64" s="111">
         <f t="shared" si="13"/>
         <v>5.0632911392405067</v>
       </c>
@@ -17964,10 +17874,10 @@
       <c r="D65">
         <v>145.5</v>
       </c>
-      <c r="E65" s="119">
+      <c r="E65" s="112">
         <v>106.2</v>
       </c>
-      <c r="F65" s="119">
+      <c r="F65" s="112">
         <f t="shared" si="10"/>
         <v>39.299999999999997</v>
       </c>
@@ -17975,11 +17885,11 @@
         <f t="shared" si="11"/>
         <v>19.649999999999999</v>
       </c>
-      <c r="H65" s="118">
+      <c r="H65" s="111">
         <f t="shared" si="12"/>
         <v>0.19650000000000001</v>
       </c>
-      <c r="I65" s="118">
+      <c r="I65" s="111">
         <f t="shared" si="13"/>
         <v>5.0890585241730282</v>
       </c>
@@ -17991,10 +17901,10 @@
       <c r="D66">
         <v>145.5</v>
       </c>
-      <c r="E66" s="119">
+      <c r="E66" s="112">
         <v>105.5</v>
       </c>
-      <c r="F66" s="119">
+      <c r="F66" s="112">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
@@ -18002,11 +17912,11 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="H66" s="118">
+      <c r="H66" s="111">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="I66" s="118">
+      <c r="I66" s="111">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
@@ -18018,10 +17928,10 @@
       <c r="D67">
         <v>145.5</v>
       </c>
-      <c r="E67" s="119">
+      <c r="E67" s="112">
         <v>68.400000000000006</v>
       </c>
-      <c r="F67" s="119">
+      <c r="F67" s="112">
         <f t="shared" si="10"/>
         <v>77.099999999999994</v>
       </c>
@@ -18029,11 +17939,11 @@
         <f t="shared" si="11"/>
         <v>19.274999999999999</v>
       </c>
-      <c r="H67" s="118">
+      <c r="H67" s="111">
         <f t="shared" si="12"/>
         <v>0.19275</v>
       </c>
-      <c r="I67" s="118">
+      <c r="I67" s="111">
         <f t="shared" si="13"/>
         <v>5.1880674448767836</v>
       </c>
@@ -18045,10 +17955,10 @@
       <c r="D68">
         <v>145.5</v>
       </c>
-      <c r="E68" s="119">
+      <c r="E68" s="112">
         <v>67.7</v>
       </c>
-      <c r="F68" s="119">
+      <c r="F68" s="112">
         <f t="shared" si="10"/>
         <v>77.8</v>
       </c>
@@ -18056,11 +17966,11 @@
         <f t="shared" si="11"/>
         <v>19.45</v>
       </c>
-      <c r="H68" s="118">
+      <c r="H68" s="111">
         <f t="shared" si="12"/>
         <v>0.19450000000000001</v>
       </c>
-      <c r="I68" s="118">
+      <c r="I68" s="111">
         <f t="shared" si="13"/>
         <v>5.1413881748071981</v>
       </c>
@@ -18072,10 +17982,10 @@
       <c r="D69">
         <v>145.5</v>
       </c>
-      <c r="E69" s="119">
+      <c r="E69" s="112">
         <v>67.7</v>
       </c>
-      <c r="F69" s="119">
+      <c r="F69" s="112">
         <f t="shared" si="10"/>
         <v>77.8</v>
       </c>
@@ -18083,11 +17993,11 @@
         <f t="shared" si="11"/>
         <v>19.45</v>
       </c>
-      <c r="H69" s="118">
+      <c r="H69" s="111">
         <f t="shared" si="12"/>
         <v>0.19450000000000001</v>
       </c>
-      <c r="I69" s="118">
+      <c r="I69" s="111">
         <f t="shared" si="13"/>
         <v>5.1413881748071981</v>
       </c>
@@ -18099,10 +18009,10 @@
       <c r="D70">
         <v>145.5</v>
       </c>
-      <c r="E70" s="119">
+      <c r="E70" s="112">
         <v>66.8</v>
       </c>
-      <c r="F70" s="119">
+      <c r="F70" s="112">
         <f t="shared" si="10"/>
         <v>78.7</v>
       </c>
@@ -18110,11 +18020,11 @@
         <f t="shared" si="11"/>
         <v>19.675000000000001</v>
       </c>
-      <c r="H70" s="118">
+      <c r="H70" s="111">
         <f t="shared" si="12"/>
         <v>0.19675000000000001</v>
       </c>
-      <c r="I70" s="118">
+      <c r="I70" s="111">
         <f t="shared" si="13"/>
         <v>5.082592121982211</v>
       </c>
@@ -18126,10 +18036,10 @@
       <c r="D71">
         <v>145.5</v>
       </c>
-      <c r="E71" s="119">
+      <c r="E71" s="112">
         <v>66.400000000000006</v>
       </c>
-      <c r="F71" s="119">
+      <c r="F71" s="112">
         <f t="shared" si="10"/>
         <v>79.099999999999994</v>
       </c>
@@ -18137,49 +18047,49 @@
         <f t="shared" si="11"/>
         <v>19.774999999999999</v>
       </c>
-      <c r="H71" s="118">
+      <c r="H71" s="111">
         <f t="shared" si="12"/>
         <v>0.19775000000000001</v>
       </c>
-      <c r="I71" s="118">
+      <c r="I71" s="111">
         <f>C71/(F71*10)</f>
         <v>5.0568900126422252</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>112</v>
-      </c>
-      <c r="D74" s="119">
+        <v>111</v>
+      </c>
+      <c r="D74" s="112">
         <f>MAX(F57:F61)-MIN(F57:F61)</f>
         <v>8.8000000000000114</v>
       </c>
       <c r="E74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="119">
+        <v>113</v>
+      </c>
+      <c r="D75" s="112">
         <f>MAX(F62:F66)-MIN(F62:F66)</f>
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>115</v>
-      </c>
-      <c r="D76" s="119">
+        <v>114</v>
+      </c>
+      <c r="D76" s="112">
         <f>MAX(F67:F71)-MIN(F67:F71)</f>
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -18296,35 +18206,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18612,27 +18493,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F80F839-78EF-4FF4-A673-3CC84279C232}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18651,4 +18541,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>